<commit_message>
implemented form for preparation of param form
</commit_message>
<xml_diff>
--- a/scratch/CWL/ATAC-seq.cwl.job_templ.xlsx
+++ b/scratch/CWL/ATAC-seq.cwl.job_templ.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="parameters" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="configs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="config" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -63,7 +63,7 @@
     <t>37</t>
   </si>
   <si>
-    <t># CWL: config</t>
+    <t># type: config</t>
   </si>
   <si>
     <t>parameter_name</t>

</xml_diff>